<commit_message>
remove mode from analysis answer template
</commit_message>
<xml_diff>
--- a/assignments/analysis-answer-template.xlsx
+++ b/assignments/analysis-answer-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/thornbur_ad_unc_edu/Documents/course material/570-data/2020 Spring Data Reporting/MEJO570-Spring2020/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/thornbur_ad_unc_edu/Documents/Teaching/570-data/2020 Spring Data Reporting/MEJO570-Spring2020/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{53829322-7AED-A343-9BDD-20EA3F4006BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74043AD8-9E84-014F-8BED-591106D449B2}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{53829322-7AED-A343-9BDD-20EA3F4006BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D4479BB-2D12-9643-93D3-B0AEA1DDD56F}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="820" windowWidth="13020" windowHeight="15260" activeTab="2" xr2:uid="{1ACCBBD0-9D33-2542-9ABA-BBBF268D4B5F}"/>
+    <workbookView xWindow="16960" yWindow="820" windowWidth="13020" windowHeight="15260" xr2:uid="{1ACCBBD0-9D33-2542-9ABA-BBBF268D4B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Month" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>January</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Median donation</t>
-  </si>
-  <si>
-    <t>Most common donation</t>
   </si>
   <si>
     <t>Percent of total</t>
@@ -468,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4644E99-7781-814C-AF72-917C9EE0F577}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,11 +536,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -551,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C472FB4B-B9E3-9F47-8EE6-CB862C26877D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,11 +602,6 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -622,10 +609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1634E2C8-2029-2044-A78F-D82B6ED27741}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,8 +653,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -679,11 +666,6 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>